<commit_message>
My module updates with logs
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelData.xlsx
+++ b/src/test/resources/TestData/ExcelData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rakhy\eclipse-workspace-new\DsalgoTestNg\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F0E9CE-825B-4070-A3B9-7E1658981D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56D421A-058E-48AD-9573-868E32AD4AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Logindetails" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Username</t>
   </si>
@@ -57,60 +57,64 @@
     <t>test</t>
   </si>
   <si>
-    <t xml:space="preserve">def search(lst, value):
+    <t>NameError: name 'hello' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>Error occurred during submission</t>
+  </si>
+  <si>
+    <t>NameError: name 'test' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>Element Found
+Not Found</t>
+  </si>
+  <si>
+    <t>Submission Successful</t>
+  </si>
+  <si>
+    <t>techteam</t>
+  </si>
+  <si>
+    <t>Time4team$</t>
+  </si>
+  <si>
+    <t>QAteam@12</t>
+  </si>
+  <si>
+    <t>ExpectedAlert</t>
+  </si>
+  <si>
+    <t>ExpectedResult</t>
+  </si>
+  <si>
+    <t>SubmitionMessage</t>
+  </si>
+  <si>
+    <t>AlertMessage</t>
+  </si>
+  <si>
+    <t>def search(lst, value):
     # Check if the value is in the list
     if value in lst:
         return "Element Found"
-    else:
-        return "Not Found"
+    return "Not Found"
 # Example Usage
 input_list = [12, 23, 45, 67, 6, 90]
 value_to_search = 12
 print(search(input_list, value_to_search))  # Output: Element Found
 value_to_search = 25
-print(search(input_list, value_to_search))  # Output: Not Found
-</t>
-  </si>
-  <si>
-    <t>NameError: name 'hello' is not defined on line 1</t>
-  </si>
-  <si>
-    <t>output</t>
-  </si>
-  <si>
-    <t>Error occurred during submission</t>
-  </si>
-  <si>
-    <t>NameError: name 'test' is not defined on line 1</t>
-  </si>
-  <si>
-    <t>Element Found
-Not Found</t>
-  </si>
-  <si>
-    <t>Submission Successful</t>
-  </si>
-  <si>
-    <t>techteam</t>
-  </si>
-  <si>
-    <t>Time4team$</t>
-  </si>
-  <si>
-    <t>QAteam@12</t>
-  </si>
-  <si>
-    <t>ExpectedAlert</t>
-  </si>
-  <si>
-    <t>ExpectedResult</t>
+print(search(input_list, value_to_search))  # Output: Not Found</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -137,11 +141,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial Unicode MS"/>
     </font>
     <font>
       <sz val="10"/>
@@ -191,26 +190,23 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -433,15 +429,15 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="27.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13">
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,36 +448,36 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="B3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -500,36 +496,36 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -547,53 +543,56 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.26953125" customWidth="1"/>
     <col min="2" max="2" width="38.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.26953125" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>